<commit_message>
PROS-13075 - CCRU - POS KPI 2020 change
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2020/KPIs for DB - Benchmark 2020.xlsx
+++ b/Projects/CCRU/Data/KPIs_2020/KPIs for DB - Benchmark 2020.xlsx
@@ -43,43 +43,43 @@
     <t xml:space="preserve">Benchmark 2020</t>
   </si>
   <si>
+    <t xml:space="preserve">CCH coolers quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH coolers quality (Prime Pos/Max15/Merch STD/Occupancy/Lights&amp;chilled)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH products present in Customers menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH shelf share in Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH shelf share in Juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH shelf share in SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH shelf share in Tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH shelf share in Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of CCH activation points in NARTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of CCH cooler doors and/or equivalent in Customer coolers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of CCH displays points of interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of NCB core assortment available in-store</t>
+  </si>
+  <si>
     <t xml:space="preserve">Number of SSD core assortment available in-store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of NCB core assortment available in-store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH shelf share in SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH shelf share in Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH shelf share in Juice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH shelf share in Tea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH shelf share in Energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of CCH displays points of interaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of CCH cooler doors and-or equivalent in Customer coolers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH coolers quality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH products present in Customers menu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of CCH activation points in NARTD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH coolers quality (Prime Pos/Max15/Merch STD/Occupancy/Lights&amp;chilled)</t>
   </si>
 </sst>
 </file>
@@ -199,16 +199,16 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.080971659919"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="67.0688259109312"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6801619433198"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="61"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,7 +471,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>6</v>
       </c>

</xml_diff>